<commit_message>
Updated Claiming testcases as per latest release.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ClaimingTestData.xlsx
+++ b/src/test/test-data/ClaimingTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>GET</t>
   </si>
@@ -58,18 +58,9 @@
     <t>status=200</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>Content-Type=application/json</t>
-  </si>
-  <si>
     <t>1PCLAIMING</t>
   </si>
   <si>
-    <t>Verify that authors of claimed article returned using API</t>
-  </si>
-  <si>
     <t>OPQA-896</t>
   </si>
   <si>
@@ -88,100 +79,13 @@
     <t>hits.hits[0]._id||hits.hits[1]._id</t>
   </si>
   <si>
-    <t>/claiming/(OPQA-896_hits.hits[0]._id)/authors</t>
-  </si>
-  <si>
-    <t>OPQA-AAA</t>
-  </si>
-  <si>
-    <t>Verify that user claims an article for the given author truid</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/article</t>
-  </si>
-  <si>
-    <t>OPQA-BBB</t>
-  </si>
-  <si>
-    <t>Verify that user unclaims an article for the given author truid</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/articles</t>
-  </si>
-  <si>
-    <t>Verify that author details returned for the given author truid</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/author</t>
-  </si>
-  <si>
-    <t>status=400</t>
-  </si>
-  <si>
-    <t>Verify that count of claimed articles returned for the given author truid</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/count/article</t>
-  </si>
-  <si>
-    <t>Verify that authorized ORCIDs are returned for the given author truid</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/orcid/auth</t>
-  </si>
-  <si>
-    <t>OPQA-CCC</t>
-  </si>
-  <si>
-    <t>OPQA-DDD</t>
-  </si>
-  <si>
-    <t>OPQA-EEE</t>
-  </si>
-  <si>
-    <t>OPQA-FFF</t>
-  </si>
-  <si>
     <t>OPQA-GGG</t>
   </si>
   <si>
-    <t>{"authorName":"Project Neon1","ut":"13014795WOS15"}</t>
-  </si>
-  <si>
-    <t>status=200||articleId=13014795WOS15||truid=(SYS_USER1)||ut=13014795WOS15</t>
-  </si>
-  <si>
-    <t>/claiming/(SYS_USER1)/article/13014795WOS15</t>
-  </si>
-  <si>
-    <t>status=204</t>
-  </si>
-  <si>
-    <t>Verify that all claimed articles returned for the given author truid</t>
-  </si>
-  <si>
-    <t>status=200||articles[0].articleId=13014795WOS15||articles[0].truid=(SYS_USER1)||articles[0].ut=13014795WOS15</t>
-  </si>
-  <si>
-    <t>Verify that user can't claims the claimed article for the given author truid and check the error status using API</t>
-  </si>
-  <si>
-    <t>status=409||errorMessage=This article has already been claimed by this user.</t>
-  </si>
-  <si>
-    <t>Verify that user can't unclaims the unclaimed an article for the given author truid and check the error status</t>
-  </si>
-  <si>
-    <t>status=409||errorMessage=This article has not been claimed by this user.</t>
-  </si>
-  <si>
-    <t>OPQA-HHH</t>
-  </si>
-  <si>
-    <t>OPQA-III</t>
+    <t>/claiming/(SYS_USER1)/orcid</t>
+  </si>
+  <si>
+    <t>Verify that ORCIDs are returned for the given author truid</t>
   </si>
 </sst>
 </file>
@@ -277,7 +181,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -293,7 +197,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,10 +525,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -661,23 +564,23 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2"/>
@@ -685,246 +588,36 @@
         <v>13</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="H3"/>
+      <c r="J3" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="31.5">
-      <c r="A4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="31.5">
-      <c r="A5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="31.5">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="31.5">
-      <c r="A7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="31.5">
-      <c r="A8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8"/>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9"/>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="31.5">
-      <c r="A10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="47.25">
-      <c r="A11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
-    <hyperlink ref="I3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-896"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Jira ids for STeAM test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/ClaimingTestData.xlsx
+++ b/src/test/test-data/ClaimingTestData.xlsx
@@ -79,13 +79,13 @@
     <t>hits.hits[0]._id||hits.hits[1]._id</t>
   </si>
   <si>
-    <t>OPQA-GGG</t>
-  </si>
-  <si>
     <t>/claiming/(SYS_USER1)/orcid</t>
   </si>
   <si>
     <t>Verify that ORCIDs are returned for the given author truid</t>
+  </si>
+  <si>
+    <t>OPQA-1409</t>
   </si>
 </sst>
 </file>
@@ -504,13 +504,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L2:L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -594,16 +594,16 @@
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Updated 1PSEARCHV4 dependent tests in Claiming module.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ClaimingTestData.xlsx
+++ b/src/test/test-data/ClaimingTestData.xlsx
@@ -67,9 +67,6 @@
     <t>Verify that to get articles for query</t>
   </si>
   <si>
-    <t>1PSEARCHV3</t>
-  </si>
-  <si>
     <t>/wos/search</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>OPQA-1409</t>
+  </si>
+  <si>
+    <t>1PSEARCHV4</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,17 +570,17 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
       <c r="G2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2"/>
@@ -588,22 +588,22 @@
         <v>13</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed claiming test which was skipped for storing response data
</commit_message>
<xml_diff>
--- a/src/test/test-data/ClaimingTestData.xlsx
+++ b/src/test/test-data/ClaimingTestData.xlsx
@@ -73,9 +73,6 @@
     <t>?query=biology</t>
   </si>
   <si>
-    <t>hits.hits[0]._id||hits.hits[1]._id</t>
-  </si>
-  <si>
     <t>/claiming/(SYS_USER1)/orcid</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>1PSEARCHV4</t>
+  </si>
+  <si>
+    <t>hits[0].id||hits[1].id</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>17</v>
@@ -588,22 +588,22 @@
         <v>13</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>

</xml_diff>